<commit_message>
Adding Sections 4-6 of Chapter 5.
</commit_message>
<xml_diff>
--- a/error_rates.xlsx
+++ b/error_rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\lkovacs\Stat. II. Python Jegyzet\Computational-Statistics-Lecture-Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kola1\Documents\Github Repok\Computational-Statistics-Lecture-Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4854339A-E565-4442-8AE7-E4F3FA48599C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08501CFE-853B-41C5-B316-649D7DC75A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -381,13 +381,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,7 +398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -409,7 +409,7 @@
         <v>0.874</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -420,7 +420,7 @@
         <v>0.69520000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>30</v>
       </c>
@@ -431,7 +431,7 @@
         <v>0.5292</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40</v>
       </c>
@@ -442,7 +442,7 @@
         <v>0.39179999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -453,7 +453,7 @@
         <v>0.28989999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60</v>
       </c>
@@ -464,7 +464,7 @@
         <v>0.2059</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>70</v>
       </c>
@@ -475,7 +475,7 @@
         <v>0.14960000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>80</v>
       </c>
@@ -486,7 +486,7 @@
         <v>0.1048</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>90</v>
       </c>
@@ -497,7 +497,7 @@
         <v>7.1900000000000006E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100</v>
       </c>
@@ -508,7 +508,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>110</v>
       </c>
@@ -519,7 +519,7 @@
         <v>3.4500000000000003E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>120</v>
       </c>
@@ -530,7 +530,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>200</v>
       </c>
@@ -541,7 +541,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>500</v>
       </c>
@@ -549,6 +549,28 @@
         <v>0.06</v>
       </c>
       <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1000</v>
+      </c>
+      <c r="B16">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2000</v>
+      </c>
+      <c r="B17">
+        <v>5.21E-2</v>
+      </c>
+      <c r="C17">
         <v>0</v>
       </c>
     </row>

</xml_diff>